<commit_message>
Low code/No Data Integrity Testing - Using Idaithalam (Simply using Microsoft Excel)
</commit_message>
<xml_diff>
--- a/db/src/test/resources/db/data-integrity-testing.xlsx
+++ b/db/src/test/resources/db/data-integrity-testing.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\db\src\test\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB6EBC2-66DD-4640-8A10-606C4C0B53E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B369574-BA8B-4FC7-A27C-56CE5B311B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Integrity Testing " sheetId="3" r:id="rId1"/>
+    <sheet name="Data-Integrity-Testing" sheetId="3" r:id="rId1"/>
     <sheet name="CSS-Accept-DB" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -160,6 +160,9 @@
   <si>
     <t xml:space="preserve">EMP_NO,BIRTH_DATE,FIRST_NAME,LAST_NAME,GENDER,HIRE_DATE
 i~1,1983-11-17,Danny,Ray,Male,2012-03-24          </t>
+  </si>
+  <si>
+    <t>Verify record</t>
   </si>
 </sst>
 </file>
@@ -1016,19 +1019,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A74E884-B4C5-4476-BC5B-7B07DD3CCD48}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="135.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="65.140625" customWidth="1"/>
+    <col min="7" max="7" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1057,7 +1060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
@@ -1073,7 +1076,7 @@
       <c r="E2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="15" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="14"/>
@@ -1081,7 +1084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>32</v>
       </c>
@@ -1097,7 +1100,7 @@
       <c r="E3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="14"/>
@@ -1105,7 +1108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>36</v>
       </c>
@@ -1116,12 +1119,12 @@
         <v>27</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="15" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="15" t="s">
@@ -1142,7 +1145,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated with tag to classify  examples
</commit_message>
<xml_diff>
--- a/db/src/test/resources/db/data-integrity-testing.xlsx
+++ b/db/src/test/resources/db/data-integrity-testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\db\src\test\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE55F5E4-E2D7-484C-BCE5-26CCF18CDE8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923515F3-8636-4979-97EC-D2F5F89A19AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -121,10 +121,31 @@
     <t>Delete record</t>
   </si>
   <si>
-    <t xml:space="preserve">delete from employees where emp_no = 1 </t>
-  </si>
-  <si>
     <t>DELETE</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @ddl  @sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @sql-insert @sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @sql-delete @sql</t>
+  </si>
+  <si>
+    <t>StoreResponseVariables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete from employees where emp_no = [empId] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @sql-select @sql-verfiy @sql @store_sql_response</t>
+  </si>
+  <si>
+    <t>empId=[0].EMP_NO</t>
   </si>
 </sst>
 </file>
@@ -525,9 +546,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A74E884-B4C5-4476-BC5B-7B07DD3CCD48}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -540,9 +561,11 @@
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="65.140625" customWidth="1"/>
     <col min="7" max="7" width="59.7109375" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,10 +588,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -588,11 +617,15 @@
         <v>14</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -612,11 +645,15 @@
         <v>22</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -638,11 +675,17 @@
       <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="J4" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -659,11 +702,15 @@
         <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="2" t="s">
-        <v>29</v>
+      <c r="J5" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Files are little organized
</commit_message>
<xml_diff>
--- a/db/src/test/resources/db/data-integrity-testing.xlsx
+++ b/db/src/test/resources/db/data-integrity-testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\db\src\test\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923515F3-8636-4979-97EC-D2F5F89A19AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3352EA66-6EAE-4080-BA07-13F007E103DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView minimized="1" xWindow="3540" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Integrity-Testing" sheetId="3" r:id="rId1"/>
@@ -152,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,13 +170,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +198,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,14 +242,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -548,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A74E884-B4C5-4476-BC5B-7B07DD3CCD48}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,158 +583,159 @@
     <col min="2" max="2" width="4.85546875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="65.140625" customWidth="1"/>
     <col min="7" max="7" width="59.7109375" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:10" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>